<commit_message>
Cleaned up extra lines in the menu-test.xlsx file.
</commit_message>
<xml_diff>
--- a/selenium-tests/resources/data/menu-test.xlsx
+++ b/selenium-tests/resources/data/menu-test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denisputnam/git/selenium-TestNiche/selenium-tests/resources/data/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denisputnam/git/selenium-TestNiche/selenium-tests/resources/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A78B1DA-27F3-994B-95D4-E81E807943EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C96E94-3FE2-2541-995A-4718AEC7FFCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4A46C506-F1EC-4042-AD96-2984A1791A07}"/>
+    <workbookView xWindow="15860" yWindow="4320" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{4A46C506-F1EC-4042-AD96-2984A1791A07}"/>
   </bookViews>
   <sheets>
     <sheet name="OverviewTC1.0.0" sheetId="1" r:id="rId1"/>
@@ -579,10 +579,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D978F605-D76C-4622-9C9A-0A774AF0F560}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -648,12 +648,6 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>